<commit_message>
new test data commit
</commit_message>
<xml_diff>
--- a/TestData_A5_Add_to_MLI.xlsx
+++ b/TestData_A5_Add_to_MLI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Demo\Udaan_Test Automation_TestCase2_Add_To_MLI\Udaan_Test Automation_TestCase2_Add_To_MLI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEAEF2B-6004-4C8B-B670-77A15351516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215AF696-1AE3-4C54-ADC8-4C0087DAB482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,31 +36,31 @@
     <t>Status</t>
   </si>
   <si>
-    <t>uiokh</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>kdmkdfkd</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>Counter</t>
   </si>
   <si>
-    <t>LME</t>
-  </si>
-  <si>
-    <t>iodpcfjsdlc</t>
-  </si>
-  <si>
-    <t>rja</t>
-  </si>
-  <si>
-    <t>asdvbhmfcdf</t>
+    <t>TestingDemo</t>
+  </si>
+  <si>
+    <t>Tes</t>
+  </si>
+  <si>
+    <t>TestingDemoo</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>TestingD</t>
+  </si>
+  <si>
+    <t>TD</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,18 +440,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -459,13 +459,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -473,13 +473,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>3</v>

</xml_diff>

<commit_message>
New test data run
</commit_message>
<xml_diff>
--- a/TestData_A5_Add_to_MLI.xlsx
+++ b/TestData_A5_Add_to_MLI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Demo\Udaan_Test Automation_TestCase2_Add_To_MLI\Udaan_Test Automation_TestCase2_Add_To_MLI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51FDF44-A870-4EF3-BB25-FADD98F1BAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3DEDAB-6EA4-4114-BDBC-378CBF97FEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>Ver</t>
   </si>
   <si>
-    <t>Sainath</t>
-  </si>
-  <si>
     <t>Redd</t>
+  </si>
+  <si>
+    <t>Sainathh</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,10 +473,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>

</xml_diff>